<commit_message>
Data extraction draft update
From April 2020
</commit_message>
<xml_diff>
--- a/Russell Data Extraction Rose Bengal.xlsx
+++ b/Russell Data Extraction Rose Bengal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Allanna\University\2018 PhD\REVIEWS\Review 1 Rose Bengal\Data Extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E26FA2-925D-4D77-9270-7B50870889ED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8D9435-1377-46D9-8564-BB99BC48C2E0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{048E3D89-01AA-4C78-B68A-E284C4D7AA8A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="263">
   <si>
     <t>Variable name</t>
   </si>
@@ -53,6 +53,9 @@
     <t>Title</t>
   </si>
   <si>
+    <t>Diabetes</t>
+  </si>
+  <si>
     <t>Strain</t>
   </si>
   <si>
@@ -74,6 +77,9 @@
     <t>Contact</t>
   </si>
   <si>
+    <t>Comorbidities</t>
+  </si>
+  <si>
     <t>Author</t>
   </si>
   <si>
@@ -287,33 +293,6 @@
     <t>Cranial window</t>
   </si>
   <si>
-    <t>RB_administration_route</t>
-  </si>
-  <si>
-    <t>Intraperitoneal injection</t>
-  </si>
-  <si>
-    <t>Intravenous injection</t>
-  </si>
-  <si>
-    <t>Venous catheter</t>
-  </si>
-  <si>
-    <t>Arterial catheter</t>
-  </si>
-  <si>
-    <t>RB_administration_time</t>
-  </si>
-  <si>
-    <t>Before light illumination</t>
-  </si>
-  <si>
-    <t>After light illumination</t>
-  </si>
-  <si>
-    <t>Same time as light illumination</t>
-  </si>
-  <si>
     <t>Light_type</t>
   </si>
   <si>
@@ -386,16 +365,10 @@
     <t>Text (drop down menu)</t>
   </si>
   <si>
-    <t>Whether the dye was administered before, during, or after illumination</t>
-  </si>
-  <si>
     <t>not sure if needed</t>
   </si>
   <si>
     <t>The type of laser light used to induce Rose Bengal Stroke</t>
-  </si>
-  <si>
-    <t>How the Rose Bengal dye was administered (tail vein injection, intraperitoneal injection etc)</t>
   </si>
   <si>
     <t>If the stroke was induced in an awake animal (such as through a cranial window) the anaesthetic will be listed as "none"</t>
@@ -559,9 +532,6 @@
     <t>Xylazene</t>
   </si>
   <si>
-    <t>Should this list be the same as O'Collins? Define as I go?</t>
-  </si>
-  <si>
     <t>mm3</t>
   </si>
   <si>
@@ -821,6 +791,63 @@
   </si>
   <si>
     <t>Missing animal ages</t>
+  </si>
+  <si>
+    <t>Light_intensity</t>
+  </si>
+  <si>
+    <t>Light_intensity_units</t>
+  </si>
+  <si>
+    <t>The units used when describing laser intensity</t>
+  </si>
+  <si>
+    <t>The intensity of the laser/light used to induce stroke</t>
+  </si>
+  <si>
+    <t>mW/cm2</t>
+  </si>
+  <si>
+    <t>If the animals being studied had any disease comorbidities such as high blood pressure, diabetes, etc.</t>
+  </si>
+  <si>
+    <t>Hypertension</t>
+  </si>
+  <si>
+    <t>Note: all SHR rats have hypertension as a comorbidity</t>
+  </si>
+  <si>
+    <t>Excitotoxicity</t>
+  </si>
+  <si>
+    <t>Anti-oxidants</t>
+  </si>
+  <si>
+    <t>Blood flow</t>
+  </si>
+  <si>
+    <t>Fluid regulation</t>
+  </si>
+  <si>
+    <t>Unsure</t>
+  </si>
+  <si>
+    <t>Anti-inflammation</t>
+  </si>
+  <si>
+    <t>Energy substrates</t>
+  </si>
+  <si>
+    <t>Anti-apoptosis/regeneration</t>
+  </si>
+  <si>
+    <t>Thrombolytics</t>
+  </si>
+  <si>
+    <t>Nootropics/cognition</t>
+  </si>
+  <si>
+    <t>mW</t>
   </si>
 </sst>
 </file>
@@ -988,7 +1015,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1028,6 +1055,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1345,13 +1373,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E976DFA-0C5F-420E-B56E-FCE6088B9022}">
-  <dimension ref="A1:BB19"/>
+  <dimension ref="A1:BC19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1363,58 +1391,58 @@
     <col min="5" max="5" width="12.33203125" customWidth="1"/>
     <col min="6" max="6" width="15.21875" customWidth="1"/>
     <col min="7" max="7" width="12.77734375" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" style="18" customWidth="1"/>
-    <col min="10" max="10" width="16" style="18" customWidth="1"/>
-    <col min="11" max="11" width="14.44140625" style="18" customWidth="1"/>
-    <col min="12" max="12" width="13.5546875" style="18" customWidth="1"/>
-    <col min="13" max="13" width="14.88671875" style="18" customWidth="1"/>
-    <col min="14" max="14" width="13.6640625" style="18" customWidth="1"/>
-    <col min="15" max="15" width="18.6640625" customWidth="1"/>
-    <col min="16" max="16" width="19.77734375" customWidth="1"/>
-    <col min="17" max="17" width="18" customWidth="1"/>
-    <col min="18" max="18" width="18.6640625" customWidth="1"/>
-    <col min="19" max="19" width="21.6640625" customWidth="1"/>
-    <col min="20" max="20" width="18.33203125" customWidth="1"/>
-    <col min="21" max="21" width="14.21875" customWidth="1"/>
-    <col min="22" max="22" width="11" customWidth="1"/>
-    <col min="23" max="23" width="13.6640625" customWidth="1"/>
-    <col min="24" max="24" width="21.77734375" customWidth="1"/>
-    <col min="25" max="25" width="22.33203125" customWidth="1"/>
-    <col min="26" max="26" width="11.5546875" customWidth="1"/>
-    <col min="27" max="27" width="10.109375" customWidth="1"/>
-    <col min="28" max="28" width="11" customWidth="1"/>
-    <col min="29" max="29" width="17.77734375" customWidth="1"/>
-    <col min="30" max="30" width="20.44140625" customWidth="1"/>
-    <col min="31" max="31" width="15" customWidth="1"/>
-    <col min="32" max="32" width="15.77734375" customWidth="1"/>
-    <col min="33" max="33" width="15.44140625" customWidth="1"/>
-    <col min="34" max="36" width="20.21875" customWidth="1"/>
-    <col min="37" max="37" width="23.109375" customWidth="1"/>
-    <col min="38" max="38" width="20.21875" customWidth="1"/>
-    <col min="39" max="39" width="20.44140625" customWidth="1"/>
-    <col min="40" max="40" width="18.6640625" customWidth="1"/>
-    <col min="41" max="41" width="19.5546875" customWidth="1"/>
-    <col min="42" max="42" width="21.88671875" customWidth="1"/>
-    <col min="43" max="43" width="21.21875" customWidth="1"/>
-    <col min="44" max="44" width="22.109375" customWidth="1"/>
-    <col min="45" max="45" width="12.44140625" customWidth="1"/>
-    <col min="46" max="46" width="16.77734375" customWidth="1"/>
-    <col min="47" max="47" width="11.88671875" customWidth="1"/>
-    <col min="48" max="48" width="18.6640625" customWidth="1"/>
-    <col min="49" max="49" width="15.6640625" customWidth="1"/>
-    <col min="50" max="50" width="21.109375" customWidth="1"/>
-    <col min="51" max="51" width="18.77734375" customWidth="1"/>
-    <col min="52" max="52" width="20.44140625" customWidth="1"/>
-    <col min="53" max="53" width="28.88671875" customWidth="1"/>
-    <col min="54" max="54" width="14.77734375" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" style="18" customWidth="1"/>
+    <col min="11" max="11" width="16" style="18" customWidth="1"/>
+    <col min="12" max="12" width="14.44140625" style="18" customWidth="1"/>
+    <col min="13" max="13" width="13.5546875" style="18" customWidth="1"/>
+    <col min="14" max="14" width="14.88671875" style="18" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" style="18" customWidth="1"/>
+    <col min="16" max="16" width="18.6640625" customWidth="1"/>
+    <col min="17" max="17" width="19.77734375" customWidth="1"/>
+    <col min="18" max="18" width="18" customWidth="1"/>
+    <col min="19" max="19" width="18.6640625" customWidth="1"/>
+    <col min="20" max="20" width="21.6640625" customWidth="1"/>
+    <col min="21" max="21" width="18.33203125" customWidth="1"/>
+    <col min="22" max="22" width="14.21875" customWidth="1"/>
+    <col min="23" max="23" width="11" customWidth="1"/>
+    <col min="24" max="25" width="13.6640625" customWidth="1"/>
+    <col min="26" max="26" width="18.6640625" customWidth="1"/>
+    <col min="27" max="27" width="11.5546875" customWidth="1"/>
+    <col min="28" max="28" width="10.109375" customWidth="1"/>
+    <col min="29" max="29" width="11" customWidth="1"/>
+    <col min="30" max="30" width="17.77734375" customWidth="1"/>
+    <col min="31" max="31" width="20.44140625" customWidth="1"/>
+    <col min="32" max="32" width="15" customWidth="1"/>
+    <col min="33" max="33" width="15.77734375" customWidth="1"/>
+    <col min="34" max="34" width="15.44140625" customWidth="1"/>
+    <col min="35" max="37" width="20.21875" customWidth="1"/>
+    <col min="38" max="38" width="23.109375" customWidth="1"/>
+    <col min="39" max="39" width="20.21875" customWidth="1"/>
+    <col min="40" max="40" width="20.44140625" customWidth="1"/>
+    <col min="41" max="41" width="18.6640625" customWidth="1"/>
+    <col min="42" max="42" width="19.5546875" customWidth="1"/>
+    <col min="43" max="43" width="21.88671875" customWidth="1"/>
+    <col min="44" max="44" width="21.21875" customWidth="1"/>
+    <col min="45" max="45" width="22.109375" customWidth="1"/>
+    <col min="46" max="46" width="12.44140625" customWidth="1"/>
+    <col min="47" max="47" width="16.77734375" customWidth="1"/>
+    <col min="48" max="48" width="11.88671875" customWidth="1"/>
+    <col min="49" max="49" width="18.6640625" customWidth="1"/>
+    <col min="50" max="50" width="15.6640625" customWidth="1"/>
+    <col min="51" max="51" width="21.109375" customWidth="1"/>
+    <col min="52" max="52" width="18.77734375" customWidth="1"/>
+    <col min="53" max="53" width="20.44140625" customWidth="1"/>
+    <col min="54" max="54" width="28.88671875" customWidth="1"/>
+    <col min="55" max="55" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>4</v>
@@ -1423,1232 +1451,1217 @@
         <v>5</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="11" t="s">
-        <v>200</v>
-      </c>
       <c r="J1" s="11" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="L1" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="S1" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="U1" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="V1" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="W1" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="X1" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z1" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="AA1" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB1" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC1" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AD1" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="AE1" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF1" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="AG1" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="AH1" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI1" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ1" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="AK1" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="AL1" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="M1" s="17" t="s">
-        <v>204</v>
-      </c>
-      <c r="N1" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="O1" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="R1" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="S1" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="T1" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="U1" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="V1" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="W1" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="X1" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="Y1" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z1" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="AA1" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="AB1" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="AC1" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="AD1" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="AE1" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="AF1" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="AG1" s="13" t="s">
+      <c r="AM1" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="AN1" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="AH1" s="13" t="s">
+      <c r="AO1" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="AP1" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="AQ1" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="AI1" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="AJ1" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="AK1" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="AL1" s="13" t="s">
+      <c r="AR1" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="AS1" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="AT1" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="AU1" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="AV1" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="AW1" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="AX1" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="AY1" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="AZ1" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA1" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="BB1" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="AM1" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="AN1" s="14" t="s">
-        <v>241</v>
-      </c>
-      <c r="AO1" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="AP1" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="AQ1" s="14" t="s">
-        <v>242</v>
-      </c>
-      <c r="AR1" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="AS1" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="AT1" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="AU1" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="AV1" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="AW1" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="AX1" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="AY1" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="AZ1" s="14" t="s">
+      <c r="BC1" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>160</v>
       </c>
-      <c r="BA1" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="BB1" s="15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>170</v>
-      </c>
       <c r="B2" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C2" s="2">
         <v>2004</v>
       </c>
       <c r="D2" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="E2" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="23"/>
+      <c r="J2" s="18">
+        <v>10</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="18">
+        <v>12</v>
+      </c>
+      <c r="M2" s="18">
+        <v>210</v>
+      </c>
+      <c r="N2" s="18">
+        <v>298</v>
+      </c>
+      <c r="O2" s="18">
+        <v>320</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>12</v>
+      </c>
+      <c r="R2">
+        <v>3</v>
+      </c>
+      <c r="S2">
+        <v>8</v>
+      </c>
+      <c r="T2">
+        <f t="shared" ref="T2:T3" si="0">IF(AND(P2&lt;&gt;"", P2&lt;&gt;0, P2&lt;&gt;"NA"), R2/P2, "NA")</f>
+        <v>3</v>
+      </c>
+      <c r="U2">
+        <f t="shared" ref="U2:U4" si="1">IF(AND(T2&lt;&gt;"", T2&lt;&gt;0, T2&lt;&gt;"NA"), Q2/T2, "NA")</f>
+        <v>4</v>
+      </c>
+      <c r="V2" t="s">
+        <v>81</v>
+      </c>
+      <c r="W2">
+        <v>10</v>
+      </c>
+      <c r="X2" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y2" s="23"/>
+      <c r="Z2" s="23"/>
+      <c r="AA2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AB2">
+        <v>20</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>101</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>175</v>
+      </c>
+      <c r="AG2" s="23"/>
+      <c r="AH2">
+        <v>10</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>167</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AK2">
+        <v>1</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>178</v>
+      </c>
+      <c r="AN2" s="23"/>
+      <c r="AO2" s="23"/>
+      <c r="AP2">
         <v>24</v>
       </c>
-      <c r="G2" t="s">
-        <v>174</v>
-      </c>
-      <c r="H2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="18">
-        <v>10</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="18">
+      <c r="AQ2" s="23"/>
+      <c r="AR2" s="23"/>
+      <c r="AS2">
+        <v>24</v>
+      </c>
+      <c r="AT2" s="23"/>
+      <c r="AU2" s="23"/>
+      <c r="AV2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="18">
-        <v>210</v>
-      </c>
-      <c r="M2" s="18">
-        <v>298</v>
-      </c>
-      <c r="N2" s="18">
-        <v>320</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <v>12</v>
-      </c>
-      <c r="Q2">
-        <v>3</v>
-      </c>
-      <c r="R2">
-        <v>8</v>
-      </c>
-      <c r="S2">
-        <f t="shared" ref="S2:S3" si="0">IF(AND(O2&lt;&gt;"", O2&lt;&gt;0, O2&lt;&gt;"NA"), Q2/O2, "NA")</f>
-        <v>3</v>
-      </c>
-      <c r="T2">
-        <f t="shared" ref="T2:T4" si="1">IF(AND(S2&lt;&gt;"", S2&lt;&gt;0, S2&lt;&gt;"NA"), P2/S2, "NA")</f>
-        <v>4</v>
-      </c>
-      <c r="U2" t="s">
-        <v>79</v>
-      </c>
-      <c r="V2">
-        <v>10</v>
-      </c>
-      <c r="W2" t="s">
-        <v>177</v>
-      </c>
-      <c r="X2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>178</v>
-      </c>
-      <c r="AA2">
-        <v>20</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>104</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>179</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>185</v>
-      </c>
-      <c r="AF2" s="23"/>
-      <c r="AG2">
-        <v>10</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>177</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AJ2">
-        <v>1</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>188</v>
-      </c>
-      <c r="AM2" s="23"/>
-      <c r="AN2" s="23"/>
-      <c r="AO2">
-        <v>24</v>
-      </c>
-      <c r="AP2" s="23"/>
-      <c r="AQ2" s="23"/>
-      <c r="AR2">
-        <v>24</v>
-      </c>
-      <c r="AS2" s="23"/>
-      <c r="AT2" s="23"/>
-      <c r="AU2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>7</v>
-      </c>
       <c r="AW2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AX2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AY2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AZ2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BA2" t="s">
-        <v>191</v>
+        <v>8</v>
       </c>
       <c r="BB2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C3" s="2">
         <v>2004</v>
       </c>
       <c r="D3" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="E3" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" s="18">
+        <v>38</v>
+      </c>
+      <c r="I3" s="23"/>
+      <c r="J3" s="18">
         <v>10</v>
       </c>
-      <c r="J3" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" s="18">
+      <c r="K3" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="18">
         <v>12</v>
       </c>
-      <c r="L3" s="18">
+      <c r="M3" s="18">
         <v>210</v>
       </c>
-      <c r="M3" s="18">
+      <c r="N3" s="18">
         <v>280</v>
       </c>
-      <c r="N3" s="18">
+      <c r="O3" s="18">
         <v>320</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>1</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>12</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>3</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>10</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="U3" t="s">
-        <v>79</v>
-      </c>
-      <c r="V3">
+      <c r="V3" t="s">
+        <v>81</v>
+      </c>
+      <c r="W3">
         <v>10</v>
       </c>
-      <c r="W3" t="s">
-        <v>177</v>
-      </c>
       <c r="X3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>178</v>
-      </c>
-      <c r="AA3">
+        <v>167</v>
+      </c>
+      <c r="Y3" s="23"/>
+      <c r="Z3" s="23"/>
+      <c r="AA3" t="s">
+        <v>168</v>
+      </c>
+      <c r="AB3">
         <v>20</v>
       </c>
-      <c r="AB3" t="s">
-        <v>104</v>
-      </c>
       <c r="AC3" t="s">
-        <v>179</v>
+        <v>97</v>
       </c>
       <c r="AD3" t="s">
-        <v>108</v>
+        <v>169</v>
       </c>
       <c r="AE3" t="s">
-        <v>185</v>
-      </c>
-      <c r="AF3" s="23"/>
-      <c r="AG3">
+        <v>101</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>175</v>
+      </c>
+      <c r="AG3" s="23"/>
+      <c r="AH3">
         <v>10</v>
       </c>
-      <c r="AH3" t="s">
-        <v>177</v>
-      </c>
-      <c r="AI3">
-        <v>1</v>
+      <c r="AI3" t="s">
+        <v>167</v>
       </c>
       <c r="AJ3">
         <v>1</v>
       </c>
-      <c r="AK3" t="s">
-        <v>7</v>
+      <c r="AK3">
+        <v>1</v>
       </c>
       <c r="AL3" t="s">
-        <v>190</v>
-      </c>
-      <c r="AM3" s="23"/>
+        <v>8</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>180</v>
+      </c>
       <c r="AN3" s="23"/>
-      <c r="AO3">
+      <c r="AO3" s="23"/>
+      <c r="AP3">
         <v>24</v>
       </c>
-      <c r="AP3" s="23"/>
       <c r="AQ3" s="23"/>
-      <c r="AR3">
+      <c r="AR3" s="23"/>
+      <c r="AS3">
         <v>24</v>
       </c>
-      <c r="AS3" s="23"/>
       <c r="AT3" s="23"/>
-      <c r="AU3" t="s">
-        <v>11</v>
-      </c>
+      <c r="AU3" s="23"/>
       <c r="AV3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="AW3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AX3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AY3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AZ3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C4" s="2">
         <v>2004</v>
       </c>
       <c r="D4" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="E4" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="18">
+        <v>38</v>
+      </c>
+      <c r="I4" s="23"/>
+      <c r="J4" s="18">
         <v>10</v>
       </c>
-      <c r="J4" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" s="18">
+      <c r="K4" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="18">
         <v>12</v>
       </c>
-      <c r="L4" s="18">
+      <c r="M4" s="18">
         <v>210</v>
       </c>
-      <c r="M4" s="18">
+      <c r="N4" s="18">
         <v>276</v>
       </c>
-      <c r="N4" s="18">
+      <c r="O4" s="18">
         <v>320</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>1</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>12</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>3</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>9</v>
       </c>
-      <c r="S4">
-        <f>IF(AND(O4&lt;&gt;"", O4&lt;&gt;0, O4&lt;&gt;"NA"), Q4/O4, "NA")</f>
+      <c r="T4">
+        <f>IF(AND(P4&lt;&gt;"", P4&lt;&gt;0, P4&lt;&gt;"NA"), R4/P4, "NA")</f>
         <v>3</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="U4" t="s">
-        <v>79</v>
-      </c>
-      <c r="V4">
+      <c r="V4" t="s">
+        <v>81</v>
+      </c>
+      <c r="W4">
         <v>10</v>
       </c>
-      <c r="W4" t="s">
-        <v>177</v>
-      </c>
       <c r="X4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>178</v>
-      </c>
-      <c r="AA4">
+        <v>167</v>
+      </c>
+      <c r="Y4" s="23"/>
+      <c r="Z4" s="23"/>
+      <c r="AA4" t="s">
+        <v>168</v>
+      </c>
+      <c r="AB4">
         <v>20</v>
       </c>
-      <c r="AB4" t="s">
-        <v>104</v>
-      </c>
       <c r="AC4" t="s">
-        <v>179</v>
+        <v>97</v>
       </c>
       <c r="AD4" t="s">
-        <v>108</v>
+        <v>169</v>
       </c>
       <c r="AE4" t="s">
-        <v>185</v>
-      </c>
-      <c r="AF4" s="23"/>
-      <c r="AG4">
+        <v>101</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>175</v>
+      </c>
+      <c r="AG4" s="23"/>
+      <c r="AH4">
         <v>10</v>
       </c>
-      <c r="AH4" t="s">
-        <v>177</v>
-      </c>
-      <c r="AI4">
+      <c r="AI4" t="s">
+        <v>167</v>
+      </c>
+      <c r="AJ4">
         <v>4</v>
       </c>
-      <c r="AJ4">
+      <c r="AK4">
         <v>1</v>
       </c>
-      <c r="AK4" t="s">
-        <v>7</v>
-      </c>
       <c r="AL4" t="s">
-        <v>190</v>
-      </c>
-      <c r="AM4" s="23"/>
+        <v>8</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>180</v>
+      </c>
       <c r="AN4" s="23"/>
-      <c r="AO4">
+      <c r="AO4" s="23"/>
+      <c r="AP4">
         <v>24</v>
       </c>
-      <c r="AP4" s="23"/>
       <c r="AQ4" s="23"/>
-      <c r="AR4">
+      <c r="AR4" s="23"/>
+      <c r="AS4">
         <v>24</v>
       </c>
-      <c r="AS4" s="23"/>
       <c r="AT4" s="23"/>
-      <c r="AU4" t="s">
-        <v>11</v>
-      </c>
+      <c r="AU4" s="23"/>
       <c r="AV4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="AW4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AX4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AY4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AZ4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="B5" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C5" s="2">
         <v>2016</v>
       </c>
       <c r="D5" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="E5" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="23"/>
+      <c r="J5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="18">
+        <v>200</v>
+      </c>
+      <c r="N5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="O5" s="18">
+        <v>250</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>6</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>6</v>
+      </c>
+      <c r="T5">
+        <f>IF(AND(P5&lt;&gt;"", P5&lt;&gt;0, P5&lt;&gt;"NA"), R5/P5, "NA")</f>
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <f>IF(AND(T5&lt;&gt;"", T5&lt;&gt;0, T5&lt;&gt;"NA"), Q5/T5, "NA")</f>
+        <v>6</v>
+      </c>
+      <c r="V5" t="s">
+        <v>81</v>
+      </c>
+      <c r="W5">
+        <v>0.1</v>
+      </c>
+      <c r="X5" t="s">
+        <v>197</v>
+      </c>
+      <c r="Y5" s="23"/>
+      <c r="Z5" s="23"/>
+      <c r="AA5" t="s">
+        <v>168</v>
+      </c>
+      <c r="AB5">
+        <v>15</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>198</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>199</v>
+      </c>
+      <c r="AG5" s="23"/>
+      <c r="AH5">
+        <v>0.5</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>167</v>
+      </c>
+      <c r="AJ5">
         <v>24</v>
       </c>
-      <c r="G5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="K5" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="L5" s="18">
-        <v>200</v>
-      </c>
-      <c r="M5" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="N5" s="18">
-        <v>250</v>
-      </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
-      <c r="P5">
-        <v>6</v>
-      </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-      <c r="R5">
-        <v>6</v>
-      </c>
-      <c r="S5">
-        <f>IF(AND(O5&lt;&gt;"", O5&lt;&gt;0, O5&lt;&gt;"NA"), Q5/O5, "NA")</f>
-        <v>1</v>
-      </c>
-      <c r="T5">
-        <f>IF(AND(S5&lt;&gt;"", S5&lt;&gt;0, S5&lt;&gt;"NA"), P5/S5, "NA")</f>
-        <v>6</v>
-      </c>
-      <c r="U5" t="s">
-        <v>79</v>
-      </c>
-      <c r="V5">
-        <v>0.1</v>
-      </c>
-      <c r="W5" t="s">
+      <c r="AK5">
+        <v>5</v>
+      </c>
+      <c r="AL5">
+        <v>120</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>180</v>
+      </c>
+      <c r="AN5">
+        <v>4</v>
+      </c>
+      <c r="AO5">
+        <v>0.3</v>
+      </c>
+      <c r="AP5">
+        <v>288</v>
+      </c>
+      <c r="AQ5">
+        <v>2.6</v>
+      </c>
+      <c r="AR5">
+        <v>0.2</v>
+      </c>
+      <c r="AS5">
+        <v>288</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>133</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>236</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>8</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>8</v>
+      </c>
+      <c r="BB5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" t="s">
         <v>207</v>
-      </c>
-      <c r="X5" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>178</v>
-      </c>
-      <c r="AA5">
-        <v>15</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>104</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>208</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>7</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>209</v>
-      </c>
-      <c r="AF5" s="23"/>
-      <c r="AG5">
-        <v>0.5</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>177</v>
-      </c>
-      <c r="AI5">
-        <v>24</v>
-      </c>
-      <c r="AJ5">
-        <v>5</v>
-      </c>
-      <c r="AK5">
-        <v>120</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>190</v>
-      </c>
-      <c r="AM5">
-        <v>4</v>
-      </c>
-      <c r="AN5">
-        <v>0.3</v>
-      </c>
-      <c r="AO5">
-        <v>288</v>
-      </c>
-      <c r="AP5">
-        <v>2.6</v>
-      </c>
-      <c r="AQ5">
-        <v>0.2</v>
-      </c>
-      <c r="AR5">
-        <v>288</v>
-      </c>
-      <c r="AS5" t="s">
-        <v>142</v>
-      </c>
-      <c r="AT5" t="s">
-        <v>246</v>
-      </c>
-      <c r="AU5" t="s">
-        <v>11</v>
-      </c>
-      <c r="AV5" t="s">
-        <v>7</v>
-      </c>
-      <c r="AW5" t="s">
-        <v>7</v>
-      </c>
-      <c r="AX5" t="s">
-        <v>7</v>
-      </c>
-      <c r="AY5" t="s">
-        <v>7</v>
-      </c>
-      <c r="AZ5" t="s">
-        <v>7</v>
-      </c>
-      <c r="BA5" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>216</v>
-      </c>
-      <c r="B6" t="s">
-        <v>217</v>
       </c>
       <c r="C6" s="2">
         <v>2016</v>
       </c>
       <c r="D6" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="E6" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
+        <v>209</v>
+      </c>
+      <c r="H6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="23"/>
+      <c r="J6" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="18">
+        <v>20</v>
+      </c>
+      <c r="N6" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="O6" s="18">
         <v>25</v>
       </c>
-      <c r="G6" t="s">
-        <v>219</v>
-      </c>
-      <c r="H6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="J6" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="K6" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="L6" s="18">
-        <v>20</v>
-      </c>
-      <c r="M6" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="N6" s="18">
-        <v>25</v>
-      </c>
-      <c r="O6">
+      <c r="P6">
         <v>1</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>6</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>1</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>6</v>
       </c>
-      <c r="S6">
-        <f t="shared" ref="S6:S14" si="2">IF(AND(O6&lt;&gt;"", O6&lt;&gt;0, O6&lt;&gt;"NA"), Q6/O6, "NA")</f>
+      <c r="T6">
+        <f t="shared" ref="T6:T14" si="2">IF(AND(P6&lt;&gt;"", P6&lt;&gt;0, P6&lt;&gt;"NA"), R6/P6, "NA")</f>
         <v>1</v>
       </c>
-      <c r="T6">
-        <f t="shared" ref="T6:T14" si="3">IF(AND(S6&lt;&gt;"", S6&lt;&gt;0, S6&lt;&gt;"NA"), P6/S6, "NA")</f>
+      <c r="U6">
+        <f t="shared" ref="U6:U14" si="3">IF(AND(T6&lt;&gt;"", T6&lt;&gt;0, T6&lt;&gt;"NA"), Q6/T6, "NA")</f>
         <v>6</v>
       </c>
-      <c r="U6" t="s">
-        <v>79</v>
-      </c>
-      <c r="V6">
+      <c r="V6" t="s">
+        <v>81</v>
+      </c>
+      <c r="W6">
         <v>1</v>
       </c>
-      <c r="W6" t="s">
-        <v>220</v>
-      </c>
       <c r="X6" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z6" t="s">
+        <v>210</v>
+      </c>
+      <c r="Y6" s="23"/>
+      <c r="Z6" s="23"/>
+      <c r="AA6" t="s">
+        <v>168</v>
+      </c>
+      <c r="AB6">
+        <v>15</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>211</v>
+      </c>
+      <c r="AG6" s="23"/>
+      <c r="AH6">
+        <v>3</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>212</v>
+      </c>
+      <c r="AJ6">
+        <v>-0.25</v>
+      </c>
+      <c r="AK6">
+        <v>1</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AM6" t="s">
         <v>178</v>
       </c>
-      <c r="AA6">
-        <v>15</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>104</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>7</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>221</v>
-      </c>
-      <c r="AF6" s="23"/>
-      <c r="AG6">
-        <v>3</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>222</v>
-      </c>
-      <c r="AI6">
-        <v>-0.25</v>
-      </c>
-      <c r="AJ6">
-        <v>1</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>7</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>188</v>
-      </c>
-      <c r="AM6">
+      <c r="AN6">
         <v>9</v>
       </c>
-      <c r="AN6">
+      <c r="AO6">
         <v>1.8</v>
       </c>
-      <c r="AO6">
+      <c r="AP6">
         <v>24</v>
       </c>
-      <c r="AP6">
+      <c r="AQ6">
         <v>2.5</v>
       </c>
-      <c r="AQ6">
+      <c r="AR6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AR6">
+      <c r="AS6">
         <v>24</v>
       </c>
-      <c r="AS6" t="s">
-        <v>167</v>
-      </c>
       <c r="AT6" t="s">
-        <v>245</v>
+        <v>157</v>
       </c>
       <c r="AU6" t="s">
-        <v>223</v>
-      </c>
-      <c r="AV6">
+        <v>235</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>213</v>
+      </c>
+      <c r="AW6">
         <v>0.6</v>
       </c>
-      <c r="AW6">
+      <c r="AX6">
         <v>0.2</v>
       </c>
-      <c r="AX6">
+      <c r="AY6">
         <v>0.3</v>
       </c>
-      <c r="AY6">
+      <c r="AZ6">
         <v>0.1</v>
       </c>
-      <c r="AZ6">
+      <c r="BA6">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B7" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C7" s="2">
         <v>2018</v>
       </c>
       <c r="D7" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="E7" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="23"/>
+      <c r="J7" s="18">
+        <v>18</v>
+      </c>
+      <c r="K7" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="H7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="18">
-        <v>18</v>
-      </c>
-      <c r="J7" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="K7" s="18">
+      <c r="L7" s="18">
         <v>19</v>
       </c>
-      <c r="L7" s="18">
+      <c r="M7" s="18">
         <v>375</v>
       </c>
-      <c r="M7" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="N7" s="18">
+      <c r="N7" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="O7" s="18">
         <v>477</v>
       </c>
-      <c r="O7" s="18">
+      <c r="P7" s="18">
         <v>1</v>
       </c>
-      <c r="P7" s="18">
+      <c r="Q7" s="18">
         <v>4</v>
       </c>
-      <c r="Q7" s="18">
+      <c r="R7" s="18">
         <v>1</v>
       </c>
-      <c r="R7" s="18">
+      <c r="S7" s="18">
         <v>7</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="U7" t="s">
-        <v>76</v>
-      </c>
-      <c r="V7">
+      <c r="V7" t="s">
+        <v>78</v>
+      </c>
+      <c r="W7">
         <v>10</v>
       </c>
-      <c r="W7" t="s">
-        <v>177</v>
-      </c>
       <c r="X7" t="s">
-        <v>87</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA7">
+        <v>167</v>
+      </c>
+      <c r="Y7" s="23"/>
+      <c r="Z7" s="23"/>
+      <c r="AA7" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB7">
         <v>10</v>
       </c>
-      <c r="AB7" t="s">
-        <v>106</v>
-      </c>
       <c r="AC7" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="AD7" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="AE7" t="s">
-        <v>230</v>
-      </c>
-      <c r="AF7" s="23"/>
-      <c r="AG7">
+        <v>8</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>220</v>
+      </c>
+      <c r="AG7" s="23"/>
+      <c r="AH7">
         <v>0.5</v>
       </c>
-      <c r="AH7" t="s">
-        <v>231</v>
-      </c>
-      <c r="AI7">
+      <c r="AI7" t="s">
+        <v>221</v>
+      </c>
+      <c r="AJ7">
         <v>-744</v>
       </c>
-      <c r="AJ7" t="s">
-        <v>7</v>
-      </c>
-      <c r="AK7">
+      <c r="AK7" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL7">
         <v>816</v>
       </c>
-      <c r="AL7" t="s">
-        <v>188</v>
-      </c>
-      <c r="AM7">
+      <c r="AM7" t="s">
+        <v>178</v>
+      </c>
+      <c r="AN7">
         <v>3015</v>
       </c>
-      <c r="AN7">
+      <c r="AO7">
         <v>55</v>
       </c>
-      <c r="AO7">
+      <c r="AP7">
         <v>72</v>
       </c>
-      <c r="AP7">
+      <c r="AQ7">
         <v>3549</v>
       </c>
-      <c r="AQ7">
+      <c r="AR7">
         <v>256</v>
       </c>
-      <c r="AR7">
+      <c r="AS7">
         <v>72</v>
       </c>
-      <c r="AS7" t="s">
-        <v>239</v>
-      </c>
       <c r="AT7" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="AU7" t="s">
-        <v>11</v>
+        <v>235</v>
       </c>
       <c r="AV7" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="AW7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AX7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AY7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AZ7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BA7" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="O8" s="15"/>
-      <c r="S8" t="str">
+        <v>8</v>
+      </c>
+      <c r="BB7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="P8" s="15"/>
+      <c r="T8" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="T8" t="str">
+      <c r="U8" t="str">
         <f t="shared" si="3"/>
         <v>NA</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="O9" s="15"/>
-      <c r="S9" t="str">
+    <row r="9" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="P9" s="15"/>
+      <c r="T9" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="T9" t="str">
+      <c r="U9" t="str">
         <f t="shared" si="3"/>
         <v>NA</v>
       </c>
     </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="O10" s="15"/>
-      <c r="S10" t="str">
+    <row r="10" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="P10" s="15"/>
+      <c r="T10" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="T10" t="str">
+      <c r="U10" t="str">
         <f t="shared" si="3"/>
         <v>NA</v>
       </c>
     </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="I11" s="21"/>
+    <row r="11" spans="1:55" x14ac:dyDescent="0.3">
       <c r="J11" s="21"/>
       <c r="K11" s="21"/>
       <c r="L11" s="21"/>
       <c r="M11" s="21"/>
       <c r="N11" s="21"/>
-      <c r="O11" s="15"/>
-      <c r="S11" t="str">
+      <c r="O11" s="21"/>
+      <c r="P11" s="15"/>
+      <c r="T11" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="T11" t="str">
+      <c r="U11" t="str">
         <f t="shared" si="3"/>
         <v>NA</v>
       </c>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="I12" s="21"/>
+    <row r="12" spans="1:55" x14ac:dyDescent="0.3">
       <c r="J12" s="21"/>
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
       <c r="M12" s="21"/>
       <c r="N12" s="21"/>
-      <c r="O12" s="15"/>
-      <c r="S12" t="str">
+      <c r="O12" s="21"/>
+      <c r="P12" s="15"/>
+      <c r="T12" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="T12" t="str">
+      <c r="U12" t="str">
         <f t="shared" si="3"/>
         <v>NA</v>
       </c>
     </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="I13" s="21"/>
+    <row r="13" spans="1:55" x14ac:dyDescent="0.3">
       <c r="J13" s="21"/>
       <c r="K13" s="21"/>
       <c r="L13" s="21"/>
       <c r="M13" s="21"/>
       <c r="N13" s="21"/>
-      <c r="O13" s="15"/>
-      <c r="S13" t="str">
+      <c r="O13" s="21"/>
+      <c r="P13" s="15"/>
+      <c r="T13" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="T13" t="str">
+      <c r="U13" t="str">
         <f t="shared" si="3"/>
         <v>NA</v>
       </c>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="I14" s="21"/>
+    <row r="14" spans="1:55" x14ac:dyDescent="0.3">
       <c r="J14" s="21"/>
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
       <c r="M14" s="21"/>
       <c r="N14" s="21"/>
-      <c r="O14" s="15"/>
-      <c r="S14" t="str">
+      <c r="O14" s="21"/>
+      <c r="P14" s="15"/>
+      <c r="T14" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="T14" t="str">
+      <c r="U14" t="str">
         <f t="shared" si="3"/>
         <v>NA</v>
       </c>
     </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="I15" s="21"/>
+    <row r="15" spans="1:55" x14ac:dyDescent="0.3">
       <c r="J15" s="21"/>
       <c r="K15" s="21"/>
       <c r="L15" s="21"/>
       <c r="M15" s="21"/>
       <c r="N15" s="21"/>
-      <c r="O15" s="15"/>
-    </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="I16" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="15"/>
+    </row>
+    <row r="16" spans="1:55" x14ac:dyDescent="0.3">
       <c r="J16" s="21"/>
       <c r="K16" s="21"/>
       <c r="L16" s="21"/>
       <c r="M16" s="21"/>
       <c r="N16" s="21"/>
-      <c r="O16" s="15"/>
-    </row>
-    <row r="17" spans="9:15" x14ac:dyDescent="0.3">
-      <c r="I17" s="21"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="15"/>
+    </row>
+    <row r="17" spans="10:16" x14ac:dyDescent="0.3">
       <c r="J17" s="21"/>
       <c r="K17" s="21"/>
       <c r="L17" s="21"/>
       <c r="M17" s="21"/>
       <c r="N17" s="21"/>
-      <c r="O17" s="15"/>
-    </row>
-    <row r="18" spans="9:15" x14ac:dyDescent="0.3">
-      <c r="I18" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="15"/>
+    </row>
+    <row r="18" spans="10:16" x14ac:dyDescent="0.3">
       <c r="J18" s="21"/>
       <c r="K18" s="21"/>
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
       <c r="N18" s="21"/>
-      <c r="O18" s="15"/>
-    </row>
-    <row r="19" spans="9:15" x14ac:dyDescent="0.3">
-      <c r="I19" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="15"/>
+    </row>
+    <row r="19" spans="10:16" x14ac:dyDescent="0.3">
       <c r="J19" s="21"/>
       <c r="K19" s="21"/>
       <c r="L19" s="21"/>
       <c r="M19" s="21"/>
       <c r="N19" s="21"/>
-      <c r="O19" s="15"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="16">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="17">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1DA07139-F5EE-4CF2-A111-554AF3F09C1F}">
           <x14:formula1>
             <xm:f>'Data validation'!$A$8:$A$21</xm:f>
@@ -2669,81 +2682,87 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{823426FD-62C3-4B24-AB9F-FE1659BB1C28}">
           <x14:formula1>
-            <xm:f>'Data validation'!$D$8:$D$14</xm:f>
+            <xm:f>'Data validation'!$E$8:$E$14</xm:f>
           </x14:formula1>
-          <xm:sqref>U2:U1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{143EA13E-88CC-45B0-96EF-6EED04AD465E}">
-          <x14:formula1>
-            <xm:f>'Data validation'!$F$8:$F$14</xm:f>
-          </x14:formula1>
-          <xm:sqref>X2:X1048576</xm:sqref>
+          <xm:sqref>V2:V1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7BC34B2C-A838-49DF-AAE0-12C0C979CA9C}">
           <x14:formula1>
             <xm:f>'Data validation'!$H$8:$H$19</xm:f>
           </x14:formula1>
-          <xm:sqref>Z2:Z1048576</xm:sqref>
+          <xm:sqref>AA2:AA1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0E7A4A47-7A09-41FD-9EE9-87A7D3C42CED}">
           <x14:formula1>
             <xm:f>'Data validation'!$I$8:$I$14</xm:f>
           </x14:formula1>
-          <xm:sqref>AB2:AB1048576</xm:sqref>
+          <xm:sqref>AC2:AC1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C8E721C8-0E28-4849-960D-832711F87A4E}">
           <x14:formula1>
             <xm:f>'Data validation'!$J$8:$J$25</xm:f>
           </x14:formula1>
-          <xm:sqref>AC2:AD1048576</xm:sqref>
+          <xm:sqref>AD2:AE1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{764A9F5C-1F38-4D0E-8206-557212552A57}">
           <x14:formula1>
             <xm:f>'Data validation'!$O$8:$O$19</xm:f>
           </x14:formula1>
-          <xm:sqref>AS2:AS1048576</xm:sqref>
+          <xm:sqref>AT2:AT1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F7D93EAF-E719-44D1-B92E-4934233B55A0}">
           <x14:formula1>
             <xm:f>'Data validation'!$Q$8:$Q$19</xm:f>
           </x14:formula1>
-          <xm:sqref>AU2:AU1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F40E8EE3-59B6-4596-9982-8D599A456F3B}">
-          <x14:formula1>
-            <xm:f>'Data validation'!$G$8:$G$12</xm:f>
-          </x14:formula1>
-          <xm:sqref>Y2:Y1048576</xm:sqref>
+          <xm:sqref>AV2:AV1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{078762FA-C545-4C39-BBF6-70D0C373B6E7}">
           <x14:formula1>
             <xm:f>'Data validation'!$M$8:$M$19</xm:f>
           </x14:formula1>
-          <xm:sqref>AH2:AH1048576</xm:sqref>
+          <xm:sqref>AI2:AI1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{42BB75B7-96C4-4627-B2B2-8CFEDE6EBB96}">
           <x14:formula1>
             <xm:f>'Data validation'!$N$8:$N$12</xm:f>
           </x14:formula1>
-          <xm:sqref>AL2:AL1048576</xm:sqref>
+          <xm:sqref>AM2:AM1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3402CC92-FA60-475F-B43E-9740D3DDA983}">
           <x14:formula1>
             <xm:f>'Data validation'!$K$8:$K$20</xm:f>
           </x14:formula1>
-          <xm:sqref>AE2:AE1048576</xm:sqref>
+          <xm:sqref>AF2:AF1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CBC780B8-3B12-4713-BD6B-B5EDA2719780}">
           <x14:formula1>
-            <xm:f>'Data validation'!$E$8:$E$19</xm:f>
+            <xm:f>'Data validation'!$F$8:$F$19</xm:f>
           </x14:formula1>
-          <xm:sqref>W2:W1048576</xm:sqref>
+          <xm:sqref>X2:X1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{087BBA9D-AF30-4754-9342-1F539C09DC13}">
           <x14:formula1>
             <xm:f>'Data validation'!$P$8:$P$15</xm:f>
           </x14:formula1>
-          <xm:sqref>AT2:AT1048576</xm:sqref>
+          <xm:sqref>AU2:AU1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CF29E257-C6BB-4642-B5D2-98B3B3ED679F}">
+          <x14:formula1>
+            <xm:f>'Data validation'!$G$8:$G$19</xm:f>
+          </x14:formula1>
+          <xm:sqref>Z2:Z1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9BFFD235-81A2-4F2F-BC6C-144D53C16444}">
+          <x14:formula1>
+            <xm:f>'Data validation'!$D$8:$D$19</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2:I1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{668DE226-CC78-4909-82E7-E57682E8372A}">
+          <x14:formula1>
+            <xm:f>'Data validation'!$L$8:$L$20</xm:f>
+          </x14:formula1>
+          <xm:sqref>AG2:AG1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2753,10 +2772,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F9050A0-7554-40B6-A78C-B5EF6AA80B73}">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2782,35 +2801,35 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="72.599999999999994" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -2818,13 +2837,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -2832,648 +2851,654 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
-        <v>116</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
-        <v>200</v>
-      </c>
       <c r="B10" t="s">
-        <v>202</v>
+        <v>109</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>249</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B11" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="D11" s="24"/>
+        <v>222</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="B12" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="D12" s="24"/>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="B13" t="s">
-        <v>144</v>
+        <v>192</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>206</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="D13" s="24"/>
     </row>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="B14" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="D14" s="24"/>
+        <v>225</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="B15" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="D15" s="24"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
-        <v>68</v>
+        <v>195</v>
       </c>
       <c r="B16" t="s">
-        <v>202</v>
+        <v>135</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>62</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="D16" s="24"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
-        <v>70</v>
-      </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>192</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
-        <v>74</v>
-      </c>
       <c r="B22" t="s">
-        <v>116</v>
+        <v>31</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B23" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="12" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="12" t="s">
-        <v>81</v>
-      </c>
       <c r="B24" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B25" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
-        <v>89</v>
+        <v>244</v>
       </c>
       <c r="B26" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>118</v>
+        <v>247</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="B27" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" t="s">
+        <v>135</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B27" t="s">
-        <v>116</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B28" t="s">
-        <v>144</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="B29" t="s">
-        <v>116</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
-        <v>181</v>
+        <v>94</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B31" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="B32" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" t="s">
+        <v>109</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B32" t="s">
-        <v>116</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="B33" t="s">
-        <v>116</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="B34" t="s">
-        <v>144</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="E34" s="15"/>
+    </row>
+    <row r="35" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B35" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
-        <v>215</v>
+        <v>116</v>
       </c>
       <c r="B36" t="s">
-        <v>144</v>
+        <v>20</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="B37" t="s">
-        <v>29</v>
+        <v>135</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="B38" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
-        <v>186</v>
+        <v>203</v>
       </c>
       <c r="B39" t="s">
-        <v>116</v>
+        <v>31</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>187</v>
+        <v>204</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="14" t="s">
-        <v>132</v>
+      <c r="A40" s="13" t="s">
+        <v>176</v>
       </c>
       <c r="B40" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>136</v>
+        <v>177</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="14" t="s">
-        <v>241</v>
+        <v>123</v>
       </c>
       <c r="B41" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E41" s="15"/>
+        <v>127</v>
+      </c>
     </row>
     <row r="42" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">
-        <v>156</v>
+        <v>231</v>
       </c>
       <c r="B42" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>157</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="E42" s="15"/>
     </row>
     <row r="43" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="14" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="B43" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="14" t="s">
-        <v>242</v>
+        <v>125</v>
       </c>
       <c r="B44" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>138</v>
+        <v>126</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="14" t="s">
-        <v>158</v>
+        <v>232</v>
       </c>
       <c r="B45" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="B46" t="s">
+        <v>135</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B46" t="s">
-        <v>116</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="14" t="s">
-        <v>249</v>
+        <v>141</v>
       </c>
       <c r="B47" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="14" t="s">
-        <v>151</v>
+        <v>239</v>
       </c>
       <c r="B48" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>152</v>
+        <v>240</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A49" s="14" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B49" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>153</v>
+        <v>143</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="14" t="s">
-        <v>247</v>
+        <v>136</v>
       </c>
       <c r="B50" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="14" t="s">
-        <v>147</v>
+        <v>237</v>
       </c>
       <c r="B51" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="14" t="s">
-        <v>248</v>
+        <v>138</v>
       </c>
       <c r="B52" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="14" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="B53" t="s">
-        <v>116</v>
+        <v>31</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A54" s="14" t="s">
-        <v>160</v>
+        <v>242</v>
       </c>
       <c r="B54" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>162</v>
+        <v>240</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A55" s="15" t="s">
-        <v>196</v>
+      <c r="A55" s="14" t="s">
+        <v>151</v>
       </c>
       <c r="B55" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>197</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="15" t="s">
-        <v>12</v>
+        <v>186</v>
       </c>
       <c r="B56" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>198</v>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A57" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="D14:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3484,22 +3509,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8607F93-07CD-454B-AFAB-DD47DEB7283E}">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.77734375" customWidth="1"/>
     <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="4" max="5" width="23.6640625" customWidth="1"/>
-    <col min="6" max="6" width="24.5546875" customWidth="1"/>
-    <col min="7" max="7" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="5" max="7" width="23.6640625" customWidth="1"/>
     <col min="8" max="8" width="12.44140625" customWidth="1"/>
     <col min="9" max="9" width="25.88671875" customWidth="1"/>
     <col min="10" max="10" width="20.33203125" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="17.44140625" customWidth="1"/>
+    <col min="12" max="12" width="24.5546875" customWidth="1"/>
     <col min="13" max="14" width="20.5546875" customWidth="1"/>
     <col min="15" max="16" width="16.44140625" customWidth="1"/>
     <col min="17" max="17" width="15.44140625" customWidth="1"/>
@@ -3507,471 +3531,496 @@
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>74</v>
-      </c>
       <c r="E6" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>245</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G8" t="s">
-        <v>90</v>
+        <v>9</v>
       </c>
       <c r="H8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" t="s">
         <v>8</v>
       </c>
       <c r="M8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="P8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Q8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>79</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>81</v>
       </c>
       <c r="F9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>92</v>
+        <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K9" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="L9" t="s">
+        <v>252</v>
       </c>
       <c r="M9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="P9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>220</v>
+        <v>78</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>210</v>
       </c>
       <c r="G10" t="s">
-        <v>91</v>
+        <v>248</v>
       </c>
       <c r="H10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I10" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="J10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="K10" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="L10" t="s">
+        <v>257</v>
       </c>
       <c r="M10" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="N10" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="O10" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="P10" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="Q10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
       <c r="D11" t="s">
-        <v>77</v>
+        <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>207</v>
+        <v>79</v>
       </c>
       <c r="F11" t="s">
-        <v>85</v>
+        <v>197</v>
       </c>
       <c r="G11" t="s">
-        <v>8</v>
+        <v>262</v>
       </c>
       <c r="H11" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="I11" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="J11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K11" t="s">
-        <v>164</v>
+        <v>155</v>
+      </c>
+      <c r="L11" t="s">
+        <v>258</v>
       </c>
       <c r="M11" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="N11" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="O11" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="P11" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="Q11" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
+        <v>250</v>
       </c>
       <c r="E12" t="s">
-        <v>177</v>
+        <v>85</v>
       </c>
       <c r="F12" t="s">
-        <v>86</v>
-      </c>
-      <c r="G12" t="s">
-        <v>7</v>
+        <v>167</v>
       </c>
       <c r="H12" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="I12" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="J12" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="K12" t="s">
-        <v>185</v>
-      </c>
-      <c r="L12" s="8"/>
+        <v>175</v>
+      </c>
+      <c r="L12" t="s">
+        <v>253</v>
+      </c>
       <c r="M12" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="N12" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="O12" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="P12" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="Q12" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" t="s">
-        <v>87</v>
+        <v>50</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
       </c>
       <c r="H13" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="I13" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="J13" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="K13" t="s">
-        <v>209</v>
-      </c>
-      <c r="L13" s="8"/>
+        <v>199</v>
+      </c>
+      <c r="L13" t="s">
+        <v>259</v>
+      </c>
       <c r="O13" s="22" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="P13" s="22"/>
       <c r="Q13" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" t="s">
-        <v>88</v>
+        <v>52</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
       </c>
       <c r="H14" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="I14" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="J14" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="K14" t="s">
-        <v>221</v>
-      </c>
-      <c r="L14" s="8"/>
+        <v>211</v>
+      </c>
+      <c r="L14" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H15" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="J15" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="K15" t="s">
-        <v>230</v>
-      </c>
-      <c r="L15" s="8"/>
+        <v>220</v>
+      </c>
+      <c r="L15" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H16" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="J16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L16" s="8"/>
+        <v>198</v>
+      </c>
+      <c r="L16" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="J17" t="s">
-        <v>112</v>
-      </c>
-      <c r="L17" s="8"/>
+        <v>105</v>
+      </c>
+      <c r="L17" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="J18" t="s">
-        <v>113</v>
+        <v>106</v>
+      </c>
+      <c r="L18" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="J19" t="s">
-        <v>114</v>
+        <v>107</v>
+      </c>
+      <c r="L19" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J20" t="s">
-        <v>165</v>
+        <v>156</v>
+      </c>
+      <c r="L20" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J21" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L24"/>
       <c r="M24"/>
       <c r="N24"/>
     </row>
@@ -3980,11 +4029,11 @@
     </row>
     <row r="31" spans="1:17" ht="288" x14ac:dyDescent="0.3">
       <c r="O31" s="4" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="P31" s="4"/>
       <c r="Q31" s="20" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>